<commit_message>
Fixed JSON to excel conversion, renamed files
</commit_message>
<xml_diff>
--- a/Formatted-Data/safety_security_and_fire_reports.xlsx
+++ b/Formatted-Data/safety_security_and_fire_reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\Formatted-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FD6278-C2CC-4D89-A4B3-D3783B12ACFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D359197-A920-4908-A63A-63F84A8ADDC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
   </bookViews>
@@ -508,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B93501D-9FFD-431F-A6B0-5767EF8CA38F}">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:F44"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
     <col min="2" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -554,14 +554,11 @@
       <c r="L1">
         <v>2018</v>
       </c>
-      <c r="M1">
-        <v>2019</v>
-      </c>
-      <c r="N1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -586,11 +583,11 @@
       <c r="K2">
         <v>317</v>
       </c>
-      <c r="N2" t="s">
+      <c r="M2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -616,7 +613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -641,11 +638,11 @@
       <c r="K4">
         <v>1722</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -671,7 +668,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -697,7 +694,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -734,14 +731,11 @@
       <c r="L8">
         <v>2018</v>
       </c>
-      <c r="M8">
-        <v>2019</v>
-      </c>
-      <c r="N8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -776,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -811,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -846,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -881,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -915,11 +909,11 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="N13" t="s">
+      <c r="M13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -953,11 +947,11 @@
       <c r="K14">
         <v>2</v>
       </c>
-      <c r="N14" t="s">
+      <c r="M14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -992,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1027,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1061,11 +1055,11 @@
       <c r="K17">
         <v>27</v>
       </c>
-      <c r="N17" t="s">
+      <c r="M17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1100,7 +1094,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1135,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1170,7 +1164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1240,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1275,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1310,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1345,7 +1339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1380,7 +1374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1415,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1450,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1520,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1555,7 +1549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1589,11 +1583,11 @@
       <c r="K32">
         <v>39</v>
       </c>
-      <c r="N32" t="s">
+      <c r="M32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1627,11 +1621,11 @@
       <c r="K33">
         <v>0</v>
       </c>
-      <c r="N33" t="s">
+      <c r="M33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1665,11 +1659,11 @@
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="N34" t="s">
+      <c r="M34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1704,7 +1698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1739,7 +1733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -1774,7 +1768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1844,7 +1838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1913,14 +1907,11 @@
       <c r="L42">
         <v>2018</v>
       </c>
-      <c r="M42">
-        <v>2019</v>
-      </c>
-      <c r="N42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1952,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -1984,7 +1975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2016,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -2048,7 +2039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -2080,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -2112,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2146,14 +2137,11 @@
       <c r="L50">
         <v>2018</v>
       </c>
-      <c r="M50">
-        <v>2019</v>
-      </c>
-      <c r="N50" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -2184,11 +2172,11 @@
       <c r="K51">
         <v>0</v>
       </c>
-      <c r="N51" t="s">
+      <c r="M51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -2220,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -2252,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -2284,7 +2272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -2316,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Added police data analysis draft
</commit_message>
<xml_diff>
--- a/Formatted-Data/safety_security_and_fire_reports.xlsx
+++ b/Formatted-Data/safety_security_and_fire_reports.xlsx
@@ -536,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B93501D-9FFD-431F-A6B0-5767EF8CA38F}">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="M43" sqref="M43"/>
+      <selection pane="topLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -587,12 +587,6 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
       <c r="G2">
         <v>250</v>
       </c>
@@ -615,12 +609,6 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
       </c>
       <c r="G3">
         <v>300</v>
@@ -642,12 +630,6 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
       <c r="G4">
         <v>1769</v>
       </c>
@@ -671,52 +653,19 @@
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
       <c r="G5">
         <v>1600</v>
       </c>
       <c r="H5">
         <v>1650</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
       <c r="H6">
         <v>200</v>
-      </c>
-      <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1053,18 +1002,6 @@
       <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
-      </c>
       <c r="G17">
         <v>36</v>
       </c>
@@ -1091,18 +1028,6 @@
       <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>37</v>
-      </c>
       <c r="G18">
         <v>94</v>
       </c>
@@ -1619,18 +1544,6 @@
       <c r="B33" t="s">
         <v>28</v>
       </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" t="s">
-        <v>35</v>
-      </c>
       <c r="G33">
         <v>2</v>
       </c>
@@ -1657,18 +1570,6 @@
       <c r="B34" t="s">
         <v>29</v>
       </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" t="s">
-        <v>35</v>
-      </c>
       <c r="G34">
         <v>2</v>
       </c>
@@ -1902,6 +1803,9 @@
       <c r="A42" t="s">
         <v>21</v>
       </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
       <c r="C42">
         <v>2009</v>
       </c>
@@ -2152,6 +2056,9 @@
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
       </c>
       <c r="C50">
         <v>2009</v>

</xml_diff>